<commit_message>
Update Gantt chart to sprint-based timeline and enhance details
</commit_message>
<xml_diff>
--- a/pilot_gantt_chart.xlsx
+++ b/pilot_gantt_chart.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Pilot Gantt Chart" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Pilot Gantt Chart (Sprints)" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -78,19 +78,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1" indent="1"/>
+      <alignment vertical="top" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -468,49 +469,85 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="80" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="90" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Activity / Task</t>
+          <t>Activity / Task (Timeline)</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>June (M1)</t>
+          <t>Sprint 1 (W1-2)</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>July (M2)</t>
+          <t>Sprint 2 (W3-4)</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>August (M3)</t>
+          <t>Sprint 3 (W5-6)</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>September (M4)</t>
+          <t>Sprint 4 (W7-8)</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>October (M5)</t>
+          <t>Sprint 5 (W9-10)</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>November (M6)</t>
+          <t>Sprint 6 (W11-12)</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Sprint 7 (W13-14)</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Sprint 8 (W15-16)</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Sprint 9 (W17-18)</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Sprint 10 (W19-20)</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Sprint 11 (W21-22)</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Sprint 12 (W23-24)</t>
         </is>
       </c>
     </row>
@@ -527,27 +564,25 @@
           <t>Discovery, Analysis &amp; Planning</t>
         </is>
       </c>
-      <c r="B3" s="5" t="n"/>
-      <c r="C3" s="5" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
-        <is>
-          <t>1. Deep Dive into Existing UAT Processes &amp; Test Assets</t>
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1. Deep Dive into Existing UAT Processes &amp; Test Assets </t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
-        <is>
-          <t>2. Identify &amp; Prioritize UAT Scenarios for Automation</t>
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2. Identify &amp; Prioritize UAT Scenarios for Automation </t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
-        <is>
-          <t>3. Master BDD Tooling &amp; Methodology</t>
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3. Master BDD Tooling &amp; Methodology </t>
         </is>
       </c>
     </row>
@@ -557,27 +592,25 @@
           <t>Migration, Automation Development &amp; Initial Integration</t>
         </is>
       </c>
-      <c r="D7" s="5" t="n"/>
-      <c r="E7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
-        <is>
-          <t>4. Convert Selected UAT Scenarios to BDD (Gherkin)</t>
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4. Convert Selected UAT Scenarios to BDD (Gherkin) </t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>5. Develop Automated Test Scripts using Playwright</t>
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5. Develop Automated Test Scripts using Playwright </t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>6. Setup &amp; Test Execution in DT2 Environment</t>
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6. Setup &amp; Test Execution in DT2 Environment </t>
         </is>
       </c>
     </row>
@@ -587,34 +620,32 @@
           <t>Refinement, Reporting &amp; Knowledge Transfer Preparation</t>
         </is>
       </c>
-      <c r="F11" s="5" t="n"/>
-      <c r="G11" s="5" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>7. Iterate and Refine Automated UAT Suite</t>
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7. Iterate and Refine Automated UAT Suite </t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="inlineStr">
-        <is>
-          <t>8. Establish Automated UAT Reporting</t>
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8. Establish Automated UAT Reporting </t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="inlineStr">
-        <is>
-          <t>9. Document Best Practices &amp; Create Migration Playbook</t>
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">9. Document Best Practices &amp; Create Migration Playbook </t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="inlineStr">
-        <is>
-          <t>10. Prepare for Knowledge Sharing &amp; Team Onboarding</t>
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10. Prepare for Knowledge Sharing &amp; Team Onboarding </t>
         </is>
       </c>
     </row>
@@ -631,27 +662,25 @@
           <t>Assessment, Strategy Definition &amp; Foundational Setup</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="inlineStr">
-        <is>
-          <t>1. Baseline Current Engineering Practices &amp; CI/CD Maturity</t>
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1. Baseline Current Engineering Practices &amp; CI/CD Maturity </t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="inlineStr">
-        <is>
-          <t>2. Develop &amp; Communicate Pilot Engineering Practices Adoption Strategy</t>
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2. Develop &amp; Communicate Pilot Engineering Practices Adoption Strategy </t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="inlineStr">
-        <is>
-          <t>3. Tooling Onboarding &amp; Environment Preparation</t>
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3. Tooling Onboarding &amp; Environment Preparation </t>
         </is>
       </c>
     </row>
@@ -661,27 +690,25 @@
           <t>Implementation, Coaching &amp; CI/CD Integration</t>
         </is>
       </c>
-      <c r="D21" s="5" t="n"/>
-      <c r="E21" s="5" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="6" t="inlineStr">
-        <is>
-          <t>4. Drive Adoption of Unit Testing &amp; Developer-Led Testing</t>
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4. Drive Adoption of Unit Testing &amp; Developer-Led Testing </t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="inlineStr">
-        <is>
-          <t>5. Integrate Automated Tests into CI/CD Pipelines (GitHub Actions Focus)</t>
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5. Integrate Automated Tests into CI/CD Pipelines (GitHub Actions Focus) </t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="inlineStr">
-        <is>
-          <t>6. Establish &amp; Champion Mocking Practices (Mockito/MockFlow)</t>
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6. Establish &amp; Champion Mocking Practices (Mockito/MockFlow) </t>
         </is>
       </c>
     </row>
@@ -691,47 +718,45 @@
           <t>Optimization, Standardization &amp; Knowledge Dissemination</t>
         </is>
       </c>
-      <c r="F25" s="5" t="n"/>
-      <c r="G25" s="5" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="inlineStr">
-        <is>
-          <t>7. Refine CI/CD Pipelines (GitHub Actions) and Test Execution Efficiency</t>
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7. Refine CI/CD Pipelines (GitHub Actions) and Test Execution Efficiency </t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="inlineStr">
-        <is>
-          <t>8. Develop &amp; Document Standardized Engineering Playbooks</t>
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8. Develop &amp; Document Standardized Engineering Playbooks </t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="inlineStr">
-        <is>
-          <t>9. Facilitate Performance Profiling Setup</t>
+      <c r="A28" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">9. Facilitate Performance Profiling Setup </t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="inlineStr">
-        <is>
-          <t>10. Prepare for Scaling &amp; Knowledge Transfer</t>
+      <c r="A29" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10. Prepare for Scaling &amp; Knowledge Transfer </t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A17"/>
-    <mergeCell ref="A3"/>
-    <mergeCell ref="A21"/>
-    <mergeCell ref="A7"/>
-    <mergeCell ref="A25"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A11"/>
+    <mergeCell ref="A17:M17"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A21:M21"/>
+    <mergeCell ref="A7:M7"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A11:M11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>